<commit_message>
cleans fields from metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/clear_escapement_raw_metadata.xlsx
+++ b/data-raw/metadata/clear_escapement_raw_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-clear-adult-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1401EAC-B1BF-4EE9-B898-55EBE28EA511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD0EB68-67B1-46EE-8E0B-9CAAE1F104DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="1275" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26535" yWindow="1665" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -134,6 +134,15 @@
   </si>
   <si>
     <t>2020-01-01</t>
+  </si>
+  <si>
+    <t>Method of survey</t>
+  </si>
+  <si>
+    <t>description of spawning status based on coloration (none, energetic, spawning colors, fungus, unknown)</t>
+  </si>
+  <si>
+    <t>spawning_condition</t>
   </si>
 </sst>
 </file>
@@ -449,11 +458,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -697,9 +706,11 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="C6" s="4" t="s">
         <v>26</v>
       </c>
@@ -715,8 +726,8 @@
       <c r="I6" s="6"/>
       <c r="J6" s="5"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -731,33 +742,43 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
@@ -799,8 +820,8 @@
       <c r="I10" s="6"/>
       <c r="J10" s="5"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -827,8 +848,8 @@
       <c r="I11" s="6"/>
       <c r="J11" s="5"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="5"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -911,8 +932,8 @@
       <c r="I14" s="6"/>
       <c r="J14" s="5"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="5"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -940,7 +961,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="12"/>
-      <c r="M15" s="5"/>
+      <c r="M15" s="12"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -995,7 +1016,7 @@
       <c r="I17" s="6"/>
       <c r="J17" s="5"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="10"/>
+      <c r="L17" s="12"/>
       <c r="M17" s="5"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1013,18 +1034,18 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="5"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -1123,8 +1144,9 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="1"/>
@@ -1150,9 +1172,8 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
-      <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
       <c r="E23" s="1"/>
@@ -1320,34 +1341,34 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
+      <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-      <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
-      <c r="Z29" s="4"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
-      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="1"/>
@@ -1379,29 +1400,39 @@
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-      <c r="T31" s="1"/>
-      <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
-      <c r="Y31" s="1"/>
-      <c r="Z31" s="1"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="4"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="3"/>
       <c r="K32" s="2"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -1420,16 +1451,6 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="4"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="3"/>
       <c r="K33" s="2"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -1560,6 +1581,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="4"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -1587,7 +1609,6 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="4"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -1615,6 +1636,7 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="4"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
@@ -1642,7 +1664,6 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="4"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
@@ -2594,7 +2615,7 @@
       <c r="Z74" s="1"/>
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="1"/>
+      <c r="A75" s="4"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="2"/>
@@ -28521,18 +28542,46 @@
       <c r="Y1000" s="1"/>
       <c r="Z1000" s="1"/>
     </row>
+    <row r="1001" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1001" s="1"/>
+      <c r="B1001" s="1"/>
+      <c r="C1001" s="1"/>
+      <c r="D1001" s="2"/>
+      <c r="E1001" s="1"/>
+      <c r="F1001" s="3"/>
+      <c r="G1001" s="3"/>
+      <c r="H1001" s="3"/>
+      <c r="I1001" s="2"/>
+      <c r="J1001" s="3"/>
+      <c r="K1001" s="2"/>
+      <c r="L1001" s="3"/>
+      <c r="M1001" s="3"/>
+      <c r="N1001" s="1"/>
+      <c r="O1001" s="1"/>
+      <c r="P1001" s="1"/>
+      <c r="Q1001" s="1"/>
+      <c r="R1001" s="1"/>
+      <c r="S1001" s="1"/>
+      <c r="T1001" s="1"/>
+      <c r="U1001" s="1"/>
+      <c r="V1001" s="1"/>
+      <c r="W1001" s="1"/>
+      <c r="X1001" s="1"/>
+      <c r="Y1001" s="1"/>
+      <c r="Z1001" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C57:C1000 C33:C45 C1:C6 C8:C31" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C58:C1001 C34:C46 C1:C7 C9:C32" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E33:E1000 E1:E6 E8:E31" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E34:E1001 E1:E7 E9:E32" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F33:F1000 F1:F6 F8:F31" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F34:F1001 F1:F7 F9:F32" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H33:H1000 H1:H6 H8:H31" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H34:H1001 H1:H7 H9:H32" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
checks fields added for escapement raw
</commit_message>
<xml_diff>
--- a/data-raw/metadata/clear_escapement_raw_metadata.xlsx
+++ b/data-raw/metadata/clear_escapement_raw_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-clear-adult-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD0EB68-67B1-46EE-8E0B-9CAAE1F104DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277AE1B5-CE4F-4652-99FC-381C64DE1CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26535" yWindow="1665" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27615" yWindow="2655" windowWidth="26430" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -143,6 +143,54 @@
   </si>
   <si>
     <t>spawning_condition</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time of video footage </t>
+  </si>
+  <si>
+    <t>hh:mm:ss</t>
+  </si>
+  <si>
+    <t>00:00:00</t>
+  </si>
+  <si>
+    <t>23:59:00</t>
+  </si>
+  <si>
+    <t>adipose_clipped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if adipose fin is clipped (TRUE/FALSE) </t>
+  </si>
+  <si>
+    <t>sex of fish observed</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>ordinal</t>
+  </si>
+  <si>
+    <t>passage_direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">direction of fish passage  </t>
+  </si>
+  <si>
+    <t>viewing_condition</t>
+  </si>
+  <si>
+    <t>direction of fish observed (normal, readable, not readable, weir is flooded)</t>
+  </si>
+  <si>
+    <t>jack_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the fish is jack sized or not </t>
   </si>
 </sst>
 </file>
@@ -458,11 +506,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1007"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -620,37 +668,33 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>14</v>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="5" t="s">
+        <v>41</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>25</v>
+      <c r="K4" s="6"/>
+      <c r="L4" s="13" t="s">
+        <v>42</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="12">
-        <v>1</v>
-      </c>
-      <c r="M4" s="5">
-        <v>2</v>
+      <c r="M4" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -668,28 +712,38 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="I5" s="6"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="12">
+        <v>1</v>
+      </c>
+      <c r="M5" s="5">
+        <v>2</v>
+      </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -706,10 +760,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>26</v>
@@ -744,10 +798,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>36</v>
+      <c r="B7" s="15" t="s">
+        <v>45</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>26</v>
@@ -764,8 +818,8 @@
       <c r="I7" s="6"/>
       <c r="J7" s="5"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -780,20 +834,68 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+    </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="4"/>
+      <c r="A9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -809,19 +911,29 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="4"/>
+      <c r="A10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
       <c r="J10" s="5"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -837,11 +949,21 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="4"/>
+      <c r="A11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -865,19 +987,29 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="6"/>
       <c r="J12" s="5"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="5"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -893,19 +1025,29 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="4"/>
+      <c r="A13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="6"/>
       <c r="J13" s="5"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="5"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -920,34 +1062,6 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-    </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
@@ -960,8 +1074,8 @@
       <c r="I15" s="6"/>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -988,7 +1102,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="5"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="12"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1016,8 +1130,8 @@
       <c r="I17" s="6"/>
       <c r="J17" s="5"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="5"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -1062,18 +1176,18 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="5"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1090,18 +1204,18 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="5"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1118,18 +1232,18 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1146,18 +1260,18 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="5"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1172,19 +1286,20 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="5"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -1201,18 +1316,18 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="5"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -1339,9 +1454,8 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
-      <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="1"/>
@@ -1369,30 +1483,31 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
+      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-      <c r="T30" s="4"/>
-      <c r="U30" s="4"/>
-      <c r="V30" s="4"/>
-      <c r="W30" s="4"/>
-      <c r="X30" s="4"/>
-      <c r="Y30" s="4"/>
-      <c r="Z30" s="4"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
@@ -1400,27 +1515,27 @@
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
-      <c r="X31" s="4"/>
-      <c r="Y31" s="4"/>
-      <c r="Z31" s="4"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
@@ -1451,6 +1566,16 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="4"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="3"/>
       <c r="K33" s="2"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -1526,31 +1651,30 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4"/>
-      <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
-      <c r="R36" s="1"/>
-      <c r="S36" s="1"/>
-      <c r="T36" s="1"/>
-      <c r="U36" s="1"/>
-      <c r="V36" s="1"/>
-      <c r="W36" s="1"/>
-      <c r="X36" s="1"/>
-      <c r="Y36" s="1"/>
-      <c r="Z36" s="1"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+      <c r="W36" s="4"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+      <c r="Z36" s="4"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4"/>
@@ -1558,27 +1682,27 @@
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-      <c r="S37" s="1"/>
-      <c r="T37" s="1"/>
-      <c r="U37" s="1"/>
-      <c r="V37" s="1"/>
-      <c r="W37" s="1"/>
-      <c r="X37" s="1"/>
-      <c r="Y37" s="1"/>
-      <c r="Z37" s="1"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="4"/>
+      <c r="X37" s="4"/>
+      <c r="Y37" s="4"/>
+      <c r="Z37" s="4"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4"/>
@@ -1609,15 +1733,6 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="3"/>
       <c r="K39" s="2"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
@@ -1664,6 +1779,7 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="4"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
@@ -1775,7 +1891,6 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="4"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="2"/>
@@ -1831,7 +1946,6 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="4"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="2"/>
@@ -2643,7 +2757,7 @@
       <c r="Z75" s="1"/>
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="1"/>
+      <c r="A76" s="4"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="2"/>
@@ -2671,7 +2785,7 @@
       <c r="Z76" s="1"/>
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="1"/>
+      <c r="A77" s="4"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="2"/>
@@ -2699,7 +2813,7 @@
       <c r="Z77" s="1"/>
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="1"/>
+      <c r="A78" s="4"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="2"/>
@@ -2727,7 +2841,7 @@
       <c r="Z78" s="1"/>
     </row>
     <row r="79" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="1"/>
+      <c r="A79" s="4"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="2"/>
@@ -2755,7 +2869,7 @@
       <c r="Z79" s="1"/>
     </row>
     <row r="80" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="1"/>
+      <c r="A80" s="4"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="2"/>
@@ -2783,7 +2897,7 @@
       <c r="Z80" s="1"/>
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="1"/>
+      <c r="A81" s="4"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="2"/>
@@ -28570,18 +28684,186 @@
       <c r="Y1001" s="1"/>
       <c r="Z1001" s="1"/>
     </row>
+    <row r="1002" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1002" s="1"/>
+      <c r="B1002" s="1"/>
+      <c r="C1002" s="1"/>
+      <c r="D1002" s="2"/>
+      <c r="E1002" s="1"/>
+      <c r="F1002" s="3"/>
+      <c r="G1002" s="3"/>
+      <c r="H1002" s="3"/>
+      <c r="I1002" s="2"/>
+      <c r="J1002" s="3"/>
+      <c r="K1002" s="2"/>
+      <c r="L1002" s="3"/>
+      <c r="M1002" s="3"/>
+      <c r="N1002" s="1"/>
+      <c r="O1002" s="1"/>
+      <c r="P1002" s="1"/>
+      <c r="Q1002" s="1"/>
+      <c r="R1002" s="1"/>
+      <c r="S1002" s="1"/>
+      <c r="T1002" s="1"/>
+      <c r="U1002" s="1"/>
+      <c r="V1002" s="1"/>
+      <c r="W1002" s="1"/>
+      <c r="X1002" s="1"/>
+      <c r="Y1002" s="1"/>
+      <c r="Z1002" s="1"/>
+    </row>
+    <row r="1003" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
+      <c r="C1003" s="1"/>
+      <c r="D1003" s="2"/>
+      <c r="E1003" s="1"/>
+      <c r="F1003" s="3"/>
+      <c r="G1003" s="3"/>
+      <c r="H1003" s="3"/>
+      <c r="I1003" s="2"/>
+      <c r="J1003" s="3"/>
+      <c r="K1003" s="2"/>
+      <c r="L1003" s="3"/>
+      <c r="M1003" s="3"/>
+      <c r="N1003" s="1"/>
+      <c r="O1003" s="1"/>
+      <c r="P1003" s="1"/>
+      <c r="Q1003" s="1"/>
+      <c r="R1003" s="1"/>
+      <c r="S1003" s="1"/>
+      <c r="T1003" s="1"/>
+      <c r="U1003" s="1"/>
+      <c r="V1003" s="1"/>
+      <c r="W1003" s="1"/>
+      <c r="X1003" s="1"/>
+      <c r="Y1003" s="1"/>
+      <c r="Z1003" s="1"/>
+    </row>
+    <row r="1004" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1004" s="1"/>
+      <c r="B1004" s="1"/>
+      <c r="C1004" s="1"/>
+      <c r="D1004" s="2"/>
+      <c r="E1004" s="1"/>
+      <c r="F1004" s="3"/>
+      <c r="G1004" s="3"/>
+      <c r="H1004" s="3"/>
+      <c r="I1004" s="2"/>
+      <c r="J1004" s="3"/>
+      <c r="K1004" s="2"/>
+      <c r="L1004" s="3"/>
+      <c r="M1004" s="3"/>
+      <c r="N1004" s="1"/>
+      <c r="O1004" s="1"/>
+      <c r="P1004" s="1"/>
+      <c r="Q1004" s="1"/>
+      <c r="R1004" s="1"/>
+      <c r="S1004" s="1"/>
+      <c r="T1004" s="1"/>
+      <c r="U1004" s="1"/>
+      <c r="V1004" s="1"/>
+      <c r="W1004" s="1"/>
+      <c r="X1004" s="1"/>
+      <c r="Y1004" s="1"/>
+      <c r="Z1004" s="1"/>
+    </row>
+    <row r="1005" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1005" s="1"/>
+      <c r="B1005" s="1"/>
+      <c r="C1005" s="1"/>
+      <c r="D1005" s="2"/>
+      <c r="E1005" s="1"/>
+      <c r="F1005" s="3"/>
+      <c r="G1005" s="3"/>
+      <c r="H1005" s="3"/>
+      <c r="I1005" s="2"/>
+      <c r="J1005" s="3"/>
+      <c r="K1005" s="2"/>
+      <c r="L1005" s="3"/>
+      <c r="M1005" s="3"/>
+      <c r="N1005" s="1"/>
+      <c r="O1005" s="1"/>
+      <c r="P1005" s="1"/>
+      <c r="Q1005" s="1"/>
+      <c r="R1005" s="1"/>
+      <c r="S1005" s="1"/>
+      <c r="T1005" s="1"/>
+      <c r="U1005" s="1"/>
+      <c r="V1005" s="1"/>
+      <c r="W1005" s="1"/>
+      <c r="X1005" s="1"/>
+      <c r="Y1005" s="1"/>
+      <c r="Z1005" s="1"/>
+    </row>
+    <row r="1006" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1006" s="1"/>
+      <c r="B1006" s="1"/>
+      <c r="C1006" s="1"/>
+      <c r="D1006" s="2"/>
+      <c r="E1006" s="1"/>
+      <c r="F1006" s="3"/>
+      <c r="G1006" s="3"/>
+      <c r="H1006" s="3"/>
+      <c r="I1006" s="2"/>
+      <c r="J1006" s="3"/>
+      <c r="K1006" s="2"/>
+      <c r="L1006" s="3"/>
+      <c r="M1006" s="3"/>
+      <c r="N1006" s="1"/>
+      <c r="O1006" s="1"/>
+      <c r="P1006" s="1"/>
+      <c r="Q1006" s="1"/>
+      <c r="R1006" s="1"/>
+      <c r="S1006" s="1"/>
+      <c r="T1006" s="1"/>
+      <c r="U1006" s="1"/>
+      <c r="V1006" s="1"/>
+      <c r="W1006" s="1"/>
+      <c r="X1006" s="1"/>
+      <c r="Y1006" s="1"/>
+      <c r="Z1006" s="1"/>
+    </row>
+    <row r="1007" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1007" s="1"/>
+      <c r="B1007" s="1"/>
+      <c r="C1007" s="1"/>
+      <c r="D1007" s="2"/>
+      <c r="E1007" s="1"/>
+      <c r="F1007" s="3"/>
+      <c r="G1007" s="3"/>
+      <c r="H1007" s="3"/>
+      <c r="I1007" s="2"/>
+      <c r="J1007" s="3"/>
+      <c r="K1007" s="2"/>
+      <c r="L1007" s="3"/>
+      <c r="M1007" s="3"/>
+      <c r="N1007" s="1"/>
+      <c r="O1007" s="1"/>
+      <c r="P1007" s="1"/>
+      <c r="Q1007" s="1"/>
+      <c r="R1007" s="1"/>
+      <c r="S1007" s="1"/>
+      <c r="T1007" s="1"/>
+      <c r="U1007" s="1"/>
+      <c r="V1007" s="1"/>
+      <c r="W1007" s="1"/>
+      <c r="X1007" s="1"/>
+      <c r="Y1007" s="1"/>
+      <c r="Z1007" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C58:C1001 C34:C46 C1:C7 C9:C32" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C64:C1007 C40:C52 C1:C13 C15:C38" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E34:E1001 E1:E7 E9:E32" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E40:E1007 E15:E38 E1:E13" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F34:F1001 F1:F7 F9:F32" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F40:F1007 F1:F13 F15:F38" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H34:H1001 H1:H7 H9:H32" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H40:H1007 H1:H13 H15:H38" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>